<commit_message>
updates to app list
</commit_message>
<xml_diff>
--- a/inst/extdata/shinyap-branches.xlsx
+++ b/inst/extdata/shinyap-branches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjfrigaard/projects/pkgs/shinyap/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjfrigaard/projects/pkgs/shinypak/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C71B1F78-C5D8-404C-903C-8472334891DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F6765-4BE4-0947-BF16-651FE0D7C871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{BDADAA3F-E15F-F14D-819C-072944368C52}"/>
+    <workbookView xWindow="4480" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{BDADAA3F-E15F-F14D-819C-072944368C52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t>01_whole-app-game</t>
   </si>
@@ -95,45 +95,6 @@
     <t>14_tests-system</t>
   </si>
   <si>
-    <t>18_golem</t>
-  </si>
-  <si>
-    <t>19_leprechaun</t>
-  </si>
-  <si>
-    <t>20_rhino</t>
-  </si>
-  <si>
-    <t>21.1_debugging</t>
-  </si>
-  <si>
-    <t>21.2_debugging</t>
-  </si>
-  <si>
-    <t>21.3_debugging</t>
-  </si>
-  <si>
-    <t>21.4_debugging</t>
-  </si>
-  <si>
-    <t>21.5_debugging</t>
-  </si>
-  <si>
-    <t>22.1_reactive-values</t>
-  </si>
-  <si>
-    <t>22.2_user-data</t>
-  </si>
-  <si>
-    <t>23_tests-snapshots</t>
-  </si>
-  <si>
-    <t>24_tests-mocks</t>
-  </si>
-  <si>
-    <t>st_trace-matrix</t>
-  </si>
-  <si>
     <t>branch</t>
   </si>
   <si>
@@ -158,12 +119,6 @@
     <t>15_docker</t>
   </si>
   <si>
-    <t>16_cicd</t>
-  </si>
-  <si>
-    <t>17_code_tools</t>
-  </si>
-  <si>
     <t>Frameworks</t>
   </si>
   <si>
@@ -224,9 +179,6 @@
     <t>CI/CD</t>
   </si>
   <si>
-    <t>Code tools</t>
-  </si>
-  <si>
     <t>golem</t>
   </si>
   <si>
@@ -242,13 +194,94 @@
     <t>Values vs. data</t>
   </si>
   <si>
-    <t>Graph snapshots</t>
-  </si>
-  <si>
-    <t>Test mocks</t>
-  </si>
-  <si>
-    <t>Traceability Matrix</t>
+    <t>16.1_cicd-style</t>
+  </si>
+  <si>
+    <t>16.2_cicd-shiny</t>
+  </si>
+  <si>
+    <t>16.3_cicd-docker</t>
+  </si>
+  <si>
+    <t>17_golem</t>
+  </si>
+  <si>
+    <t>18_leprechaun</t>
+  </si>
+  <si>
+    <t>19_rhino</t>
+  </si>
+  <si>
+    <t>20_css</t>
+  </si>
+  <si>
+    <t>21_js</t>
+  </si>
+  <si>
+    <t>22_python</t>
+  </si>
+  <si>
+    <t>23.1_debug-error</t>
+  </si>
+  <si>
+    <t>23.2_debug-selected_vars</t>
+  </si>
+  <si>
+    <t>23.3_debug-var_inputs</t>
+  </si>
+  <si>
+    <t>23.4_debug-scatter_plot</t>
+  </si>
+  <si>
+    <t>23.5_debug-print</t>
+  </si>
+  <si>
+    <t>Non-R Code</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>Test mocks and snapshots</t>
+  </si>
+  <si>
+    <t>24.1.0_reactive-values</t>
+  </si>
+  <si>
+    <t>24.1.1_step_01</t>
+  </si>
+  <si>
+    <t>24.1.2_step_02</t>
+  </si>
+  <si>
+    <t>24.1.3_step_03</t>
+  </si>
+  <si>
+    <t>24.1.4_step_04</t>
+  </si>
+  <si>
+    <t>24.2_user-data</t>
+  </si>
+  <si>
+    <t>24.2.0_user-data</t>
+  </si>
+  <si>
+    <t>24.2.1_step_01</t>
+  </si>
+  <si>
+    <t>24.2.2_step_02</t>
+  </si>
+  <si>
+    <t>A.E_mocks-snapshots</t>
   </si>
 </sst>
 </file>
@@ -600,28 +633,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DFE73F-6B55-AE4F-BA95-31D077FE758B}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C48" sqref="A1:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -629,43 +662,43 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -673,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -684,10 +717,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -695,10 +728,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -706,10 +739,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -717,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -728,10 +761,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,10 +772,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -750,10 +783,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -761,10 +794,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -772,10 +805,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -783,10 +816,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -794,10 +827,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -805,10 +838,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -816,10 +849,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -827,10 +860,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -838,10 +871,10 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -849,10 +882,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -860,186 +893,285 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
         <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>